<commit_message>
Footer Added & Survey Score Removed From DB/XLSX
</commit_message>
<xml_diff>
--- a/dashboard/static/dashboard/Employee Statistics.xlsx
+++ b/dashboard/static/dashboard/Employee Statistics.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Stuff\Dissertation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Desktop\dissertation_project\dashboard\static\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E840B7-AB13-4FCE-BD27-8789577B17F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645C2015-E6EB-4F07-89C6-40C356B0BD35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Monthly Results'!$K$1:$M$2</definedName>
-    <definedName name="Data">'Monthly Results'!$B$2:$I$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Monthly Results'!$J$1:$L$2</definedName>
+    <definedName name="Data">'Monthly Results'!$B$2:$H$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Abbey</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>Tickets Closed</t>
-  </si>
-  <si>
-    <t>Average Survey Score</t>
   </si>
   <si>
     <t>Counter Queries Taken</t>
@@ -114,7 +111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,12 +127,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -215,49 +206,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,114 +539,104 @@
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <f t="shared" ref="A2:A10" si="0">RANK(I2,$I$2:$I$10)</f>
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
+        <f t="shared" ref="A2:A10" si="0">RANK(H2,$H$2:$H$10)</f>
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
         <v>93</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>38</v>
       </c>
-      <c r="E2" s="8">
-        <v>4.53</v>
-      </c>
-      <c r="F2" s="9">
+      <c r="E2" s="7">
         <v>2</v>
       </c>
-      <c r="G2" s="10">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2" s="4">
-        <f>SUM(C2:H2)-(H2*50)+(E2*10)</f>
-        <v>183.83</v>
-      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16">
+        <f>SUM(C2:G2)-(G2*50)</f>
+        <v>134</v>
+      </c>
+      <c r="I2"/>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
-      <c r="M2"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
         <v>207</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>146</v>
       </c>
-      <c r="E3" s="8">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <f t="shared" ref="I3:I10" si="1">SUM(C3:H3)-(H3*50)+(E3*10)</f>
-        <v>406.35</v>
-      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16">
+        <f t="shared" ref="H3:H10" si="1">SUM(C3:G3)-(G3*50)</f>
+        <v>353</v>
+      </c>
+      <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -670,104 +644,95 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>327</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>170</v>
       </c>
-      <c r="E4" s="8">
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>7</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="16">
         <f t="shared" si="1"/>
-        <v>499.15</v>
-      </c>
+        <v>455</v>
+      </c>
+      <c r="I4"/>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
-      <c r="M4"/>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>57</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>41</v>
       </c>
-      <c r="E5" s="8">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0</v>
-      </c>
-      <c r="G5" s="10">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="16">
         <f t="shared" si="1"/>
-        <v>103.9</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I5"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>157</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>109</v>
       </c>
-      <c r="E6" s="8">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="F6" s="9">
-        <v>1</v>
-      </c>
-      <c r="G6" s="10">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>3</v>
+      </c>
+      <c r="H6" s="16">
         <f t="shared" si="1"/>
-        <v>322.34000000000003</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="I6"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -775,34 +740,31 @@
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>69</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>41</v>
       </c>
-      <c r="E7" s="8">
-        <v>4.97</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="E7" s="7">
         <v>2</v>
       </c>
-      <c r="G7" s="10">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="F7" s="8">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
         <f t="shared" si="1"/>
-        <v>166.67</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -810,30 +772,27 @@
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>3249</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>165</v>
       </c>
-      <c r="E8" s="8">
-        <v>4.8899999999999997</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" s="7">
         <v>30</v>
       </c>
-      <c r="G8" s="10">
+      <c r="F8" s="8">
         <v>2</v>
       </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16">
         <f t="shared" si="1"/>
-        <v>3499.79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>3446</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -841,58 +800,52 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <v>1031</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>104</v>
       </c>
-      <c r="E9" s="8">
-        <v>4.68</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0</v>
-      </c>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16">
         <f t="shared" si="1"/>
-        <v>1187.48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <v>2324</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>129</v>
       </c>
-      <c r="E10" s="8">
-        <v>4.96</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="E10" s="7">
         <v>9</v>
       </c>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="11">
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
         <v>2</v>
       </c>
-      <c r="I10" s="13">
+      <c r="H10" s="16">
         <f t="shared" si="1"/>
-        <v>2419.56</v>
+        <v>2365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>